<commit_message>
Added viewer for blogs
</commit_message>
<xml_diff>
--- a/PoundPupLegacy.Convert/FormalIntermediateLevelSubdivisions.xlsx
+++ b/PoundPupLegacy.Convert/FormalIntermediateLevelSubdivisions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pd_af\source\repos\PoundPupLegacy\PoundPupLegacy.Convert\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA05345C-D194-44E3-B2D6-960EAF068EF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F053BF-D988-40D5-A1C1-4750964F1CF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9150" yWindow="6070" windowWidth="28830" windowHeight="15460" xr2:uid="{7820BEDA-216C-45D9-AF12-C83D70C48B86}"/>
+    <workbookView xWindow="1520" yWindow="1520" windowWidth="28840" windowHeight="15460" xr2:uid="{7820BEDA-216C-45D9-AF12-C83D70C48B86}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2198,7 +2198,7 @@
   <dimension ref="A1:K200"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A173" workbookViewId="0">
-      <selection activeCell="L200" sqref="L200"/>
+      <selection activeCell="A200" sqref="A200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9178,7 +9178,7 @@
     </row>
     <row r="200" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A200">
-        <v>0</v>
+        <v>26832</v>
       </c>
       <c r="B200" s="1">
         <v>44915.741666666669</v>

</xml_diff>